<commit_message>
Luuk journal de travail
</commit_message>
<xml_diff>
--- a/documentation/3_1_Journal-Luuk-Mueller.xlsx
+++ b/documentation/3_1_Journal-Luuk-Mueller.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MuellerL15\306-G1-Piloter_un_robot_phidget_a_distance\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B7BE3F-3A8B-4904-87B0-23D7585249FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E66D3DF-B8AE-4630-AD3F-E372A7603AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
   <si>
     <t>Insérer les lignes au-dessus de celle-ci !</t>
   </si>
@@ -146,6 +146,27 @@
   </si>
   <si>
     <t>Aujourd'hui, j'ai commencé à corriger et à améliorer le kanban et le product backlog, ce qui m'a montré à quel point il est important d'avoir un kanban pour ne jamais perdre de vue le projet et toujours savoir sur quoi on travaille afin de savoir quoi faire dans les moments stressants. L'après-midi, j'ai principalement travaillé sur le frontend, où nous avons rencontré des problèmes pendant la journée, mais que nous avons finalement pu résoudre avec une autre page html temporaire. Au cours de la journée, j'ai effectué des tests pendant environ 30 minutes, qui nous ont apporté des informations importantes sur la fonctionnalité de l'application.</t>
+  </si>
+  <si>
+    <t>Développement de la page pour conduire le rover au clavier</t>
+  </si>
+  <si>
+    <t>Dévélopper la page du clavier</t>
+  </si>
+  <si>
+    <t>Fait la page pour choisir entre clavier et manette</t>
+  </si>
+  <si>
+    <t>Merge entre dashboard et le reste</t>
+  </si>
+  <si>
+    <t>Dévélopper la page de le manette</t>
+  </si>
+  <si>
+    <t>Aujourd'hui, j'ai créé un site web permettant de contrôler le rover via le clavier. Cela m'a pris pas mal de temps, car j'ai dû attribuer un identifiant à chaque élément dans les fichiers HTML. Après quelques ajustements, tout fonctionne désormais correctement et le rover répond parfaitement aux commandes du clavier.</t>
+  </si>
+  <si>
+    <t>Aujourd'hui, j'ai bien avancé sur la création des pages de contrôle pour le rover. J'ai réussi à implémenter les deux options de contrôle, et l'intégration entre le tableau de bord et les autres pages s'est bien passée. Le plus gros défi a été de m'assurer que l'interface soit fluide et intuitive, surtout avec la gestion des choix entre clavier et manette. Tout fonctionne comme prévu, mais je dois encore tester certaines interactions pour être sûr de la stabilité.</t>
   </si>
 </sst>
 </file>
@@ -491,6 +512,62 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -523,68 +600,12 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1220,9 +1241,9 @@
   <dimension ref="A1:D84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft"/>
       <selection activeCell="A5" sqref="A5:XFD5"/>
-      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
+      <selection pane="bottomLeft" activeCell="A48" sqref="A48:A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1235,85 +1256,85 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
     </row>
     <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="15"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="29"/>
       <c r="D2" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="18"/>
+      <c r="C4" s="32"/>
       <c r="D4" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="19"/>
+      <c r="A5" s="31"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="33"/>
       <c r="D5" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="20">
+      <c r="A6" s="34">
         <v>45996</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="23"/>
+      <c r="C6" s="36"/>
       <c r="D6" s="7">
         <v>3.2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="21"/>
-      <c r="B7" s="24" t="s">
+      <c r="A7" s="15"/>
+      <c r="B7" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="25"/>
+      <c r="C7" s="20"/>
       <c r="D7" s="8">
         <v>0.3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="21"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="25"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="20"/>
       <c r="D8" s="8"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="21"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="25"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="20"/>
       <c r="D9" s="8"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="21"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="25"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="20"/>
       <c r="D10" s="8"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="21"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
@@ -1326,59 +1347,59 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="21"/>
-      <c r="B12" s="26" t="s">
+      <c r="A12" s="15"/>
+      <c r="B12" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="28"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="26"/>
     </row>
     <row r="13" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="29">
+      <c r="A13" s="14">
         <v>46003</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="31"/>
+      <c r="C13" s="18"/>
       <c r="D13" s="7">
         <v>2.5</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="21"/>
-      <c r="B14" s="24" t="s">
+      <c r="A14" s="15"/>
+      <c r="B14" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="25"/>
+      <c r="C14" s="20"/>
       <c r="D14" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="21"/>
-      <c r="B15" s="24" t="s">
+      <c r="A15" s="15"/>
+      <c r="B15" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="25"/>
+      <c r="C15" s="20"/>
       <c r="D15" s="8">
         <v>3.5</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="21"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="25"/>
+      <c r="A16" s="15"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="20"/>
       <c r="D16" s="8"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="21"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="25"/>
+      <c r="A17" s="15"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="20"/>
       <c r="D17" s="8"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="21"/>
+      <c r="A18" s="15"/>
       <c r="B18" s="2" t="s">
         <v>6</v>
       </c>
@@ -1391,55 +1412,55 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="21"/>
-      <c r="B19" s="26" t="s">
+      <c r="A19" s="15"/>
+      <c r="B19" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="27"/>
-      <c r="D19" s="28"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="26"/>
     </row>
     <row r="20" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="29">
+      <c r="A20" s="14">
         <v>46009</v>
       </c>
-      <c r="B20" s="30" t="s">
+      <c r="B20" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="31"/>
+      <c r="C20" s="18"/>
       <c r="D20" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="21"/>
-      <c r="B21" s="24" t="s">
+      <c r="A21" s="15"/>
+      <c r="B21" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="25"/>
+      <c r="C21" s="20"/>
       <c r="D21" s="8">
         <v>2.5</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="21"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="25"/>
+      <c r="A22" s="15"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="20"/>
       <c r="D22" s="8"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="21"/>
-      <c r="B23" s="24"/>
-      <c r="C23" s="25"/>
+      <c r="A23" s="15"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="20"/>
       <c r="D23" s="8"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="21"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="25"/>
+      <c r="A24" s="15"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="20"/>
       <c r="D24" s="8"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="21"/>
+      <c r="A25" s="15"/>
       <c r="B25" s="2" t="s">
         <v>6</v>
       </c>
@@ -1452,63 +1473,63 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="21"/>
-      <c r="B26" s="26" t="s">
+      <c r="A26" s="15"/>
+      <c r="B26" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="27"/>
-      <c r="D26" s="28"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="26"/>
     </row>
     <row r="27" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="29">
+      <c r="A27" s="14">
         <v>46010</v>
       </c>
-      <c r="B27" s="30" t="s">
+      <c r="B27" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="31"/>
+      <c r="C27" s="18"/>
       <c r="D27" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="21"/>
-      <c r="B28" s="24" t="s">
+      <c r="A28" s="15"/>
+      <c r="B28" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="25"/>
+      <c r="C28" s="20"/>
       <c r="D28" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="21"/>
-      <c r="B29" s="24" t="s">
+      <c r="A29" s="15"/>
+      <c r="B29" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="25"/>
+      <c r="C29" s="20"/>
       <c r="D29" s="8">
         <v>3.5</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="21"/>
-      <c r="B30" s="24" t="s">
+      <c r="A30" s="15"/>
+      <c r="B30" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="25"/>
+      <c r="C30" s="20"/>
       <c r="D30" s="8">
         <v>0.5</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="21"/>
-      <c r="B31" s="24"/>
-      <c r="C31" s="25"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="20"/>
       <c r="D31" s="8"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="21"/>
+      <c r="A32" s="15"/>
       <c r="B32" s="2" t="s">
         <v>6</v>
       </c>
@@ -1521,45 +1542,47 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="98.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="32"/>
-      <c r="B33" s="33" t="s">
+      <c r="A33" s="16"/>
+      <c r="B33" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="34"/>
-      <c r="D33" s="35"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="23"/>
     </row>
     <row r="34" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="29"/>
-      <c r="B34" s="30"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="7"/>
+      <c r="A34" s="14">
+        <v>46030</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" s="18"/>
+      <c r="D34" s="7">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="21"/>
-      <c r="B35" s="24"/>
-      <c r="C35" s="25"/>
+      <c r="A35" s="15"/>
       <c r="D35" s="8"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="21"/>
-      <c r="B36" s="24"/>
-      <c r="C36" s="25"/>
+      <c r="A36" s="15"/>
       <c r="D36" s="8"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="21"/>
-      <c r="B37" s="24"/>
-      <c r="C37" s="25"/>
+      <c r="A37" s="15"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="20"/>
       <c r="D37" s="8"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="21"/>
-      <c r="B38" s="24"/>
-      <c r="C38" s="25"/>
+      <c r="A38" s="15"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="20"/>
       <c r="D38" s="8"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="21"/>
+      <c r="A39" s="15"/>
       <c r="B39" s="2" t="s">
         <v>6</v>
       </c>
@@ -1568,47 +1591,67 @@
       </c>
       <c r="D39" s="9">
         <f>SUM(D34:D38)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="32"/>
-      <c r="B40" s="33"/>
-      <c r="C40" s="34"/>
-      <c r="D40" s="35"/>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="16"/>
+      <c r="B40" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C40" s="22"/>
+      <c r="D40" s="23"/>
     </row>
     <row r="41" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="29"/>
-      <c r="B41" s="30"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="7"/>
+      <c r="A41" s="14">
+        <v>46031</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C41" s="18"/>
+      <c r="D41" s="7">
+        <v>4</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="21"/>
-      <c r="B42" s="24"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="8"/>
+      <c r="A42" s="15"/>
+      <c r="B42" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C42" s="20"/>
+      <c r="D42" s="8">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="21"/>
-      <c r="B43" s="24"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="8"/>
+      <c r="A43" s="15"/>
+      <c r="B43" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C43" s="20"/>
+      <c r="D43" s="8">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="21"/>
-      <c r="B44" s="24"/>
-      <c r="C44" s="25"/>
-      <c r="D44" s="8"/>
+      <c r="A44" s="15"/>
+      <c r="B44" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C44" s="18"/>
+      <c r="D44" s="8">
+        <v>2</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="21"/>
-      <c r="B45" s="24"/>
-      <c r="C45" s="25"/>
+      <c r="A45" s="15"/>
+      <c r="B45" s="19"/>
+      <c r="C45" s="20"/>
       <c r="D45" s="8"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="21"/>
+      <c r="A46" s="15"/>
       <c r="B46" s="2" t="s">
         <v>6</v>
       </c>
@@ -1617,47 +1660,49 @@
       </c>
       <c r="D46" s="9">
         <f>SUM(D41:D45)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="32"/>
-      <c r="B47" s="33"/>
-      <c r="C47" s="34"/>
-      <c r="D47" s="35"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="16"/>
+      <c r="B47" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C47" s="22"/>
+      <c r="D47" s="23"/>
     </row>
     <row r="48" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="29"/>
-      <c r="B48" s="30"/>
-      <c r="C48" s="31"/>
+      <c r="A48" s="14"/>
+      <c r="B48" s="17"/>
+      <c r="C48" s="18"/>
       <c r="D48" s="7"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="21"/>
-      <c r="B49" s="24"/>
-      <c r="C49" s="25"/>
+      <c r="A49" s="15"/>
+      <c r="B49" s="19"/>
+      <c r="C49" s="20"/>
       <c r="D49" s="8"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="21"/>
-      <c r="B50" s="24"/>
-      <c r="C50" s="25"/>
+      <c r="A50" s="15"/>
+      <c r="B50" s="19"/>
+      <c r="C50" s="20"/>
       <c r="D50" s="8"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="21"/>
-      <c r="B51" s="24"/>
-      <c r="C51" s="25"/>
+      <c r="A51" s="15"/>
+      <c r="B51" s="19"/>
+      <c r="C51" s="20"/>
       <c r="D51" s="8"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="21"/>
-      <c r="B52" s="24"/>
-      <c r="C52" s="25"/>
+      <c r="A52" s="15"/>
+      <c r="B52" s="19"/>
+      <c r="C52" s="20"/>
       <c r="D52" s="8"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="21"/>
+      <c r="A53" s="15"/>
       <c r="B53" s="2" t="s">
         <v>6</v>
       </c>
@@ -1670,43 +1715,43 @@
       </c>
     </row>
     <row r="54" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="32"/>
-      <c r="B54" s="33"/>
-      <c r="C54" s="34"/>
-      <c r="D54" s="35"/>
+      <c r="A54" s="16"/>
+      <c r="B54" s="21"/>
+      <c r="C54" s="22"/>
+      <c r="D54" s="23"/>
     </row>
     <row r="55" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="29"/>
-      <c r="B55" s="30"/>
-      <c r="C55" s="31"/>
+      <c r="A55" s="14"/>
+      <c r="B55" s="17"/>
+      <c r="C55" s="18"/>
       <c r="D55" s="7"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="21"/>
-      <c r="B56" s="24"/>
-      <c r="C56" s="25"/>
+      <c r="A56" s="15"/>
+      <c r="B56" s="19"/>
+      <c r="C56" s="20"/>
       <c r="D56" s="8"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="21"/>
-      <c r="B57" s="24"/>
-      <c r="C57" s="25"/>
+      <c r="A57" s="15"/>
+      <c r="B57" s="19"/>
+      <c r="C57" s="20"/>
       <c r="D57" s="8"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="21"/>
-      <c r="B58" s="24"/>
-      <c r="C58" s="25"/>
+      <c r="A58" s="15"/>
+      <c r="B58" s="19"/>
+      <c r="C58" s="20"/>
       <c r="D58" s="8"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="21"/>
-      <c r="B59" s="24"/>
-      <c r="C59" s="25"/>
+      <c r="A59" s="15"/>
+      <c r="B59" s="19"/>
+      <c r="C59" s="20"/>
       <c r="D59" s="8"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="21"/>
+      <c r="A60" s="15"/>
       <c r="B60" s="2" t="s">
         <v>6</v>
       </c>
@@ -1719,43 +1764,43 @@
       </c>
     </row>
     <row r="61" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="32"/>
-      <c r="B61" s="33"/>
-      <c r="C61" s="34"/>
-      <c r="D61" s="35"/>
+      <c r="A61" s="16"/>
+      <c r="B61" s="21"/>
+      <c r="C61" s="22"/>
+      <c r="D61" s="23"/>
     </row>
     <row r="62" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="29"/>
-      <c r="B62" s="30"/>
-      <c r="C62" s="31"/>
+      <c r="A62" s="14"/>
+      <c r="B62" s="17"/>
+      <c r="C62" s="18"/>
       <c r="D62" s="7"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="21"/>
-      <c r="B63" s="24"/>
-      <c r="C63" s="25"/>
+      <c r="A63" s="15"/>
+      <c r="B63" s="19"/>
+      <c r="C63" s="20"/>
       <c r="D63" s="8"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="21"/>
-      <c r="B64" s="24"/>
-      <c r="C64" s="25"/>
+      <c r="A64" s="15"/>
+      <c r="B64" s="19"/>
+      <c r="C64" s="20"/>
       <c r="D64" s="8"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="21"/>
-      <c r="B65" s="24"/>
-      <c r="C65" s="25"/>
+      <c r="A65" s="15"/>
+      <c r="B65" s="19"/>
+      <c r="C65" s="20"/>
       <c r="D65" s="8"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="21"/>
-      <c r="B66" s="24"/>
-      <c r="C66" s="25"/>
+      <c r="A66" s="15"/>
+      <c r="B66" s="19"/>
+      <c r="C66" s="20"/>
       <c r="D66" s="8"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="21"/>
+      <c r="A67" s="15"/>
       <c r="B67" s="2" t="s">
         <v>6</v>
       </c>
@@ -1768,43 +1813,43 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="21"/>
-      <c r="B68" s="26"/>
-      <c r="C68" s="27"/>
-      <c r="D68" s="28"/>
+      <c r="A68" s="15"/>
+      <c r="B68" s="24"/>
+      <c r="C68" s="25"/>
+      <c r="D68" s="26"/>
     </row>
     <row r="69" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="29"/>
-      <c r="B69" s="30"/>
-      <c r="C69" s="31"/>
+      <c r="A69" s="14"/>
+      <c r="B69" s="17"/>
+      <c r="C69" s="18"/>
       <c r="D69" s="7"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="21"/>
-      <c r="B70" s="24"/>
-      <c r="C70" s="25"/>
+      <c r="A70" s="15"/>
+      <c r="B70" s="19"/>
+      <c r="C70" s="20"/>
       <c r="D70" s="8"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="21"/>
-      <c r="B71" s="24"/>
-      <c r="C71" s="25"/>
+      <c r="A71" s="15"/>
+      <c r="B71" s="19"/>
+      <c r="C71" s="20"/>
       <c r="D71" s="8"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="21"/>
-      <c r="B72" s="24"/>
-      <c r="C72" s="25"/>
+      <c r="A72" s="15"/>
+      <c r="B72" s="19"/>
+      <c r="C72" s="20"/>
       <c r="D72" s="8"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="21"/>
-      <c r="B73" s="24"/>
-      <c r="C73" s="25"/>
+      <c r="A73" s="15"/>
+      <c r="B73" s="19"/>
+      <c r="C73" s="20"/>
       <c r="D73" s="8"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="21"/>
+      <c r="A74" s="15"/>
       <c r="B74" s="2" t="s">
         <v>6</v>
       </c>
@@ -1817,43 +1862,43 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="32"/>
-      <c r="B75" s="33"/>
-      <c r="C75" s="34"/>
-      <c r="D75" s="35"/>
+      <c r="A75" s="16"/>
+      <c r="B75" s="21"/>
+      <c r="C75" s="22"/>
+      <c r="D75" s="23"/>
     </row>
     <row r="76" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="29"/>
-      <c r="B76" s="30"/>
-      <c r="C76" s="31"/>
+      <c r="A76" s="14"/>
+      <c r="B76" s="17"/>
+      <c r="C76" s="18"/>
       <c r="D76" s="7"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="21"/>
-      <c r="B77" s="24"/>
-      <c r="C77" s="25"/>
+      <c r="A77" s="15"/>
+      <c r="B77" s="19"/>
+      <c r="C77" s="20"/>
       <c r="D77" s="8"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="21"/>
-      <c r="B78" s="24"/>
-      <c r="C78" s="25"/>
+      <c r="A78" s="15"/>
+      <c r="B78" s="19"/>
+      <c r="C78" s="20"/>
       <c r="D78" s="8"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="21"/>
-      <c r="B79" s="24"/>
-      <c r="C79" s="25"/>
+      <c r="A79" s="15"/>
+      <c r="B79" s="19"/>
+      <c r="C79" s="20"/>
       <c r="D79" s="8"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="21"/>
-      <c r="B80" s="24"/>
-      <c r="C80" s="25"/>
+      <c r="A80" s="15"/>
+      <c r="B80" s="19"/>
+      <c r="C80" s="20"/>
       <c r="D80" s="8"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="21"/>
+      <c r="A81" s="15"/>
       <c r="B81" s="2" t="s">
         <v>6</v>
       </c>
@@ -1866,10 +1911,10 @@
       </c>
     </row>
     <row r="82" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="32"/>
-      <c r="B82" s="33"/>
-      <c r="C82" s="34"/>
-      <c r="D82" s="35"/>
+      <c r="A82" s="16"/>
+      <c r="B82" s="21"/>
+      <c r="C82" s="22"/>
+      <c r="D82" s="23"/>
     </row>
     <row r="83" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="11"/>
@@ -1879,90 +1924,19 @@
       </c>
       <c r="D83" s="12">
         <f>D11+D18+D25+D32+D39+D46+D53+D60+D67+D74+D81</f>
-        <v>21</v>
+        <v>31.5</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" s="36" t="s">
+      <c r="A84" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B84" s="36"/>
-      <c r="C84" s="36"/>
-      <c r="D84" s="36"/>
+      <c r="B84" s="13"/>
+      <c r="C84" s="13"/>
+      <c r="D84" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="82">
-    <mergeCell ref="A84:D84"/>
-    <mergeCell ref="A76:A82"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B82:D82"/>
-    <mergeCell ref="A69:A75"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B75:D75"/>
-    <mergeCell ref="A62:A68"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="A55:A61"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B61:D61"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="A41:A47"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="A34:A40"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="A13:A19"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B19:D19"/>
+  <mergeCells count="80">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A4:A5"/>
@@ -1974,6 +1948,75 @@
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B12:D12"/>
+    <mergeCell ref="A13:A19"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="A27:A33"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="A34:A40"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="A41:A47"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="A55:A61"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="A62:A68"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="A69:A75"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="A84:D84"/>
+    <mergeCell ref="A76:A82"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B82:D82"/>
   </mergeCells>
   <conditionalFormatting sqref="D6:D11">
     <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="Terminé">
@@ -2301,6 +2344,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="8afaa137-8a18-4908-97f4-35fc924e5a91">
@@ -2309,15 +2361,6 @@
     <TaxCatchAll xmlns="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2340,6 +2383,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8C0AFF7-6D45-4588-A3CE-0506D82134A8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1CED954-0C0B-4246-88BC-C0C5C061E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -2350,12 +2401,4 @@
     <ds:schemaRef ds:uri="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8C0AFF7-6D45-4588-A3CE-0506D82134A8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Journal de travail Luuk
</commit_message>
<xml_diff>
--- a/documentation/3_1_Journal-Luuk-Mueller.xlsx
+++ b/documentation/3_1_Journal-Luuk-Mueller.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29426"/>
   <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MuellerL15\306-G1-Piloter_un_robot_phidget_a_distance\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E66D3DF-B8AE-4630-AD3F-E372A7603AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDBCF725-EB45-4801-8DA7-BA8BE87FAFB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
   <si>
     <t>Insérer les lignes au-dessus de celle-ci !</t>
   </si>
@@ -167,6 +167,33 @@
   </si>
   <si>
     <t>Aujourd'hui, j'ai bien avancé sur la création des pages de contrôle pour le rover. J'ai réussi à implémenter les deux options de contrôle, et l'intégration entre le tableau de bord et les autres pages s'est bien passée. Le plus gros défi a été de m'assurer que l'interface soit fluide et intuitive, surtout avec la gestion des choix entre clavier et manette. Tout fonctionne comme prévu, mais je dois encore tester certaines interactions pour être sûr de la stabilité.</t>
+  </si>
+  <si>
+    <t>Implémentation des touches qui s'affichent lorsque l'utilisateur les touches.</t>
+  </si>
+  <si>
+    <t>Refactorisation du code.</t>
+  </si>
+  <si>
+    <t>Ajouter les boutons pour revenir vers la page pour choisir entre clavier et manette.</t>
+  </si>
+  <si>
+    <t>Finalisation des tests</t>
+  </si>
+  <si>
+    <t>Fait le diagramme de classe</t>
+  </si>
+  <si>
+    <t>Fait le launch.json</t>
+  </si>
+  <si>
+    <t>Fait la descente de code</t>
+  </si>
+  <si>
+    <t>L’implémentation de l’affichage des touches a permis d’améliorer significativement l’interaction utilisateur. La refactorisation a rendu le code plus clair, structuré et plus facile à maintenir. L’ajout des boutons de navigation améliore l’ergonomie générale de l’application et facilite la transition entre les modes clavier et manette.</t>
+  </si>
+  <si>
+    <t>La finalisation des tests a permis de valider le bon fonctionnement global du projet. La réalisation du diagramme de classe a clarifié l’architecture et les relations entre les composants. La configuration du launch.json et la descente de code ont amélioré la compréhension du projet et facilité le débogage et la maintenance future.</t>
   </si>
 </sst>
 </file>
@@ -512,100 +539,100 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1241,9 +1268,9 @@
   <dimension ref="A1:D84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft"/>
       <selection activeCell="A5" sqref="A5:XFD5"/>
-      <selection pane="bottomLeft" activeCell="A48" sqref="A48:A54"/>
+      <selection pane="bottomLeft" activeCell="J55" sqref="J55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1256,85 +1283,85 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
     </row>
     <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="29"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="15"/>
       <c r="D2" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="32"/>
+      <c r="C4" s="18"/>
       <c r="D4" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="31"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="33"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="19"/>
       <c r="D5" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="34">
+      <c r="A6" s="20">
         <v>45996</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="36"/>
+      <c r="C6" s="23"/>
       <c r="D6" s="7">
         <v>3.2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="15"/>
-      <c r="B7" s="19" t="s">
+      <c r="A7" s="21"/>
+      <c r="B7" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="20"/>
+      <c r="C7" s="25"/>
       <c r="D7" s="8">
         <v>0.3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="15"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="20"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="25"/>
       <c r="D8" s="8"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="15"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="20"/>
+      <c r="A9" s="21"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="25"/>
       <c r="D9" s="8"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="15"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="20"/>
+      <c r="A10" s="21"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="25"/>
       <c r="D10" s="8"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="15"/>
+      <c r="A11" s="21"/>
       <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
@@ -1347,59 +1374,59 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="15"/>
-      <c r="B12" s="24" t="s">
+      <c r="A12" s="21"/>
+      <c r="B12" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="26"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="28"/>
     </row>
     <row r="13" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="14">
+      <c r="A13" s="29">
         <v>46003</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="18"/>
+      <c r="C13" s="31"/>
       <c r="D13" s="7">
         <v>2.5</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="15"/>
-      <c r="B14" s="19" t="s">
+      <c r="A14" s="21"/>
+      <c r="B14" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="20"/>
+      <c r="C14" s="25"/>
       <c r="D14" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="15"/>
-      <c r="B15" s="19" t="s">
+      <c r="A15" s="21"/>
+      <c r="B15" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="20"/>
+      <c r="C15" s="25"/>
       <c r="D15" s="8">
         <v>3.5</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="15"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="20"/>
+      <c r="A16" s="21"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="25"/>
       <c r="D16" s="8"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="15"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="20"/>
+      <c r="A17" s="21"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="25"/>
       <c r="D17" s="8"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="15"/>
+      <c r="A18" s="21"/>
       <c r="B18" s="2" t="s">
         <v>6</v>
       </c>
@@ -1412,55 +1439,55 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="15"/>
-      <c r="B19" s="24" t="s">
+      <c r="A19" s="21"/>
+      <c r="B19" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="25"/>
-      <c r="D19" s="26"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="28"/>
     </row>
     <row r="20" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="14">
+      <c r="A20" s="29">
         <v>46009</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="18"/>
+      <c r="C20" s="31"/>
       <c r="D20" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="15"/>
-      <c r="B21" s="19" t="s">
+      <c r="A21" s="21"/>
+      <c r="B21" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="20"/>
+      <c r="C21" s="25"/>
       <c r="D21" s="8">
         <v>2.5</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="15"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="20"/>
+      <c r="A22" s="21"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="25"/>
       <c r="D22" s="8"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="15"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="20"/>
+      <c r="A23" s="21"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="25"/>
       <c r="D23" s="8"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="15"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="20"/>
+      <c r="A24" s="21"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="25"/>
       <c r="D24" s="8"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="15"/>
+      <c r="A25" s="21"/>
       <c r="B25" s="2" t="s">
         <v>6</v>
       </c>
@@ -1473,63 +1500,63 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="15"/>
-      <c r="B26" s="24" t="s">
+      <c r="A26" s="21"/>
+      <c r="B26" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="25"/>
-      <c r="D26" s="26"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="28"/>
     </row>
     <row r="27" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="14">
+      <c r="A27" s="29">
         <v>46010</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="18"/>
+      <c r="C27" s="31"/>
       <c r="D27" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="15"/>
-      <c r="B28" s="19" t="s">
+      <c r="A28" s="21"/>
+      <c r="B28" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="20"/>
+      <c r="C28" s="25"/>
       <c r="D28" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="15"/>
-      <c r="B29" s="19" t="s">
+      <c r="A29" s="21"/>
+      <c r="B29" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="20"/>
+      <c r="C29" s="25"/>
       <c r="D29" s="8">
         <v>3.5</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="15"/>
-      <c r="B30" s="19" t="s">
+      <c r="A30" s="21"/>
+      <c r="B30" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="20"/>
+      <c r="C30" s="25"/>
       <c r="D30" s="8">
         <v>0.5</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="15"/>
-      <c r="B31" s="19"/>
-      <c r="C31" s="20"/>
+      <c r="A31" s="21"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="25"/>
       <c r="D31" s="8"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="15"/>
+      <c r="A32" s="21"/>
       <c r="B32" s="2" t="s">
         <v>6</v>
       </c>
@@ -1542,47 +1569,47 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="98.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="16"/>
-      <c r="B33" s="21" t="s">
+      <c r="A33" s="32"/>
+      <c r="B33" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="22"/>
-      <c r="D33" s="23"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="35"/>
     </row>
     <row r="34" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="14">
+      <c r="A34" s="29">
         <v>46030</v>
       </c>
-      <c r="B34" s="17" t="s">
+      <c r="B34" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="18"/>
+      <c r="C34" s="31"/>
       <c r="D34" s="7">
         <v>3.5</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="15"/>
+      <c r="A35" s="21"/>
       <c r="D35" s="8"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="15"/>
+      <c r="A36" s="21"/>
       <c r="D36" s="8"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="15"/>
-      <c r="B37" s="19"/>
-      <c r="C37" s="20"/>
+      <c r="A37" s="21"/>
+      <c r="B37" s="24"/>
+      <c r="C37" s="25"/>
       <c r="D37" s="8"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="15"/>
-      <c r="B38" s="19"/>
-      <c r="C38" s="20"/>
+      <c r="A38" s="21"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="25"/>
       <c r="D38" s="8"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="15"/>
+      <c r="A39" s="21"/>
       <c r="B39" s="2" t="s">
         <v>6</v>
       </c>
@@ -1595,63 +1622,63 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="16"/>
-      <c r="B40" s="21" t="s">
+      <c r="A40" s="32"/>
+      <c r="B40" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="23"/>
+      <c r="C40" s="34"/>
+      <c r="D40" s="35"/>
     </row>
     <row r="41" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="14">
+      <c r="A41" s="29">
         <v>46031</v>
       </c>
-      <c r="B41" s="17" t="s">
+      <c r="B41" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="C41" s="18"/>
+      <c r="C41" s="31"/>
       <c r="D41" s="7">
         <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="15"/>
-      <c r="B42" s="19" t="s">
+      <c r="A42" s="21"/>
+      <c r="B42" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="C42" s="20"/>
+      <c r="C42" s="25"/>
       <c r="D42" s="8">
         <v>0.5</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="15"/>
-      <c r="B43" s="19" t="s">
+      <c r="A43" s="21"/>
+      <c r="B43" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="C43" s="20"/>
+      <c r="C43" s="25"/>
       <c r="D43" s="8">
         <v>0.5</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="15"/>
-      <c r="B44" s="17" t="s">
+      <c r="A44" s="21"/>
+      <c r="B44" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="C44" s="18"/>
+      <c r="C44" s="31"/>
       <c r="D44" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="15"/>
-      <c r="B45" s="19"/>
-      <c r="C45" s="20"/>
+      <c r="A45" s="21"/>
+      <c r="B45" s="24"/>
+      <c r="C45" s="25"/>
       <c r="D45" s="8"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="15"/>
+      <c r="A46" s="21"/>
       <c r="B46" s="2" t="s">
         <v>6</v>
       </c>
@@ -1664,45 +1691,59 @@
       </c>
     </row>
     <row r="47" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="16"/>
-      <c r="B47" s="21" t="s">
+      <c r="A47" s="32"/>
+      <c r="B47" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C47" s="22"/>
-      <c r="D47" s="23"/>
+      <c r="C47" s="34"/>
+      <c r="D47" s="35"/>
     </row>
     <row r="48" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="14"/>
-      <c r="B48" s="17"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="7"/>
+      <c r="A48" s="29">
+        <v>46037</v>
+      </c>
+      <c r="B48" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="C48" s="31"/>
+      <c r="D48" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="15"/>
-      <c r="B49" s="19"/>
-      <c r="C49" s="20"/>
-      <c r="D49" s="8"/>
+      <c r="A49" s="21"/>
+      <c r="B49" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C49" s="25"/>
+      <c r="D49" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="15"/>
-      <c r="B50" s="19"/>
-      <c r="C50" s="20"/>
-      <c r="D50" s="8"/>
+      <c r="A50" s="21"/>
+      <c r="B50" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C50" s="25"/>
+      <c r="D50" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="15"/>
-      <c r="B51" s="19"/>
-      <c r="C51" s="20"/>
+      <c r="A51" s="21"/>
+      <c r="B51" s="24"/>
+      <c r="C51" s="25"/>
       <c r="D51" s="8"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="15"/>
-      <c r="B52" s="19"/>
-      <c r="C52" s="20"/>
+      <c r="A52" s="21"/>
+      <c r="B52" s="24"/>
+      <c r="C52" s="25"/>
       <c r="D52" s="8"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="15"/>
+      <c r="A53" s="21"/>
       <c r="B53" s="2" t="s">
         <v>6</v>
       </c>
@@ -1711,47 +1752,67 @@
       </c>
       <c r="D53" s="9">
         <f>SUM(D48:D52)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="16"/>
-      <c r="B54" s="21"/>
-      <c r="C54" s="22"/>
-      <c r="D54" s="23"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="32"/>
+      <c r="B54" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C54" s="34"/>
+      <c r="D54" s="35"/>
     </row>
     <row r="55" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="14"/>
-      <c r="B55" s="17"/>
-      <c r="C55" s="18"/>
-      <c r="D55" s="7"/>
+      <c r="A55" s="29">
+        <v>46038</v>
+      </c>
+      <c r="B55" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C55" s="31"/>
+      <c r="D55" s="7">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="15"/>
-      <c r="B56" s="19"/>
-      <c r="C56" s="20"/>
-      <c r="D56" s="8"/>
+      <c r="A56" s="21"/>
+      <c r="B56" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C56" s="25"/>
+      <c r="D56" s="8">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="15"/>
-      <c r="B57" s="19"/>
-      <c r="C57" s="20"/>
-      <c r="D57" s="8"/>
+      <c r="A57" s="21"/>
+      <c r="B57" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C57" s="25"/>
+      <c r="D57" s="8">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="15"/>
-      <c r="B58" s="19"/>
-      <c r="C58" s="20"/>
-      <c r="D58" s="8"/>
+      <c r="A58" s="21"/>
+      <c r="B58" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C58" s="25"/>
+      <c r="D58" s="8">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="15"/>
-      <c r="B59" s="19"/>
-      <c r="C59" s="20"/>
+      <c r="A59" s="21"/>
+      <c r="B59" s="24"/>
+      <c r="C59" s="25"/>
       <c r="D59" s="8"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="15"/>
+      <c r="A60" s="21"/>
       <c r="B60" s="2" t="s">
         <v>6</v>
       </c>
@@ -1760,47 +1821,49 @@
       </c>
       <c r="D60" s="9">
         <f>SUM(D55:D59)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="16"/>
-      <c r="B61" s="21"/>
-      <c r="C61" s="22"/>
-      <c r="D61" s="23"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="32"/>
+      <c r="B61" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="C61" s="34"/>
+      <c r="D61" s="35"/>
     </row>
     <row r="62" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="14"/>
-      <c r="B62" s="17"/>
-      <c r="C62" s="18"/>
+      <c r="A62" s="29"/>
+      <c r="B62" s="30"/>
+      <c r="C62" s="31"/>
       <c r="D62" s="7"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="15"/>
-      <c r="B63" s="19"/>
-      <c r="C63" s="20"/>
+      <c r="A63" s="21"/>
+      <c r="B63" s="24"/>
+      <c r="C63" s="25"/>
       <c r="D63" s="8"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="15"/>
-      <c r="B64" s="19"/>
-      <c r="C64" s="20"/>
+      <c r="A64" s="21"/>
+      <c r="B64" s="24"/>
+      <c r="C64" s="25"/>
       <c r="D64" s="8"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="15"/>
-      <c r="B65" s="19"/>
-      <c r="C65" s="20"/>
+      <c r="A65" s="21"/>
+      <c r="B65" s="24"/>
+      <c r="C65" s="25"/>
       <c r="D65" s="8"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="15"/>
-      <c r="B66" s="19"/>
-      <c r="C66" s="20"/>
+      <c r="A66" s="21"/>
+      <c r="B66" s="24"/>
+      <c r="C66" s="25"/>
       <c r="D66" s="8"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="15"/>
+      <c r="A67" s="21"/>
       <c r="B67" s="2" t="s">
         <v>6</v>
       </c>
@@ -1813,43 +1876,43 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="15"/>
-      <c r="B68" s="24"/>
-      <c r="C68" s="25"/>
-      <c r="D68" s="26"/>
+      <c r="A68" s="21"/>
+      <c r="B68" s="26"/>
+      <c r="C68" s="27"/>
+      <c r="D68" s="28"/>
     </row>
     <row r="69" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="14"/>
-      <c r="B69" s="17"/>
-      <c r="C69" s="18"/>
+      <c r="A69" s="29"/>
+      <c r="B69" s="30"/>
+      <c r="C69" s="31"/>
       <c r="D69" s="7"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="15"/>
-      <c r="B70" s="19"/>
-      <c r="C70" s="20"/>
+      <c r="A70" s="21"/>
+      <c r="B70" s="24"/>
+      <c r="C70" s="25"/>
       <c r="D70" s="8"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="15"/>
-      <c r="B71" s="19"/>
-      <c r="C71" s="20"/>
+      <c r="A71" s="21"/>
+      <c r="B71" s="24"/>
+      <c r="C71" s="25"/>
       <c r="D71" s="8"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="15"/>
-      <c r="B72" s="19"/>
-      <c r="C72" s="20"/>
+      <c r="A72" s="21"/>
+      <c r="B72" s="24"/>
+      <c r="C72" s="25"/>
       <c r="D72" s="8"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="15"/>
-      <c r="B73" s="19"/>
-      <c r="C73" s="20"/>
+      <c r="A73" s="21"/>
+      <c r="B73" s="24"/>
+      <c r="C73" s="25"/>
       <c r="D73" s="8"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="15"/>
+      <c r="A74" s="21"/>
       <c r="B74" s="2" t="s">
         <v>6</v>
       </c>
@@ -1862,43 +1925,43 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="16"/>
-      <c r="B75" s="21"/>
-      <c r="C75" s="22"/>
-      <c r="D75" s="23"/>
+      <c r="A75" s="32"/>
+      <c r="B75" s="33"/>
+      <c r="C75" s="34"/>
+      <c r="D75" s="35"/>
     </row>
     <row r="76" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="14"/>
-      <c r="B76" s="17"/>
-      <c r="C76" s="18"/>
+      <c r="A76" s="29"/>
+      <c r="B76" s="30"/>
+      <c r="C76" s="31"/>
       <c r="D76" s="7"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="15"/>
-      <c r="B77" s="19"/>
-      <c r="C77" s="20"/>
+      <c r="A77" s="21"/>
+      <c r="B77" s="24"/>
+      <c r="C77" s="25"/>
       <c r="D77" s="8"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="15"/>
-      <c r="B78" s="19"/>
-      <c r="C78" s="20"/>
+      <c r="A78" s="21"/>
+      <c r="B78" s="24"/>
+      <c r="C78" s="25"/>
       <c r="D78" s="8"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="15"/>
-      <c r="B79" s="19"/>
-      <c r="C79" s="20"/>
+      <c r="A79" s="21"/>
+      <c r="B79" s="24"/>
+      <c r="C79" s="25"/>
       <c r="D79" s="8"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="15"/>
-      <c r="B80" s="19"/>
-      <c r="C80" s="20"/>
+      <c r="A80" s="21"/>
+      <c r="B80" s="24"/>
+      <c r="C80" s="25"/>
       <c r="D80" s="8"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="15"/>
+      <c r="A81" s="21"/>
       <c r="B81" s="2" t="s">
         <v>6</v>
       </c>
@@ -1911,10 +1974,10 @@
       </c>
     </row>
     <row r="82" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="16"/>
-      <c r="B82" s="21"/>
-      <c r="C82" s="22"/>
-      <c r="D82" s="23"/>
+      <c r="A82" s="32"/>
+      <c r="B82" s="33"/>
+      <c r="C82" s="34"/>
+      <c r="D82" s="35"/>
     </row>
     <row r="83" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="11"/>
@@ -1924,51 +1987,55 @@
       </c>
       <c r="D83" s="12">
         <f>D11+D18+D25+D32+D39+D46+D53+D60+D67+D74+D81</f>
-        <v>31.5</v>
+        <v>41.5</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" s="13" t="s">
+      <c r="A84" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B84" s="13"/>
-      <c r="C84" s="13"/>
-      <c r="D84" s="13"/>
+      <c r="B84" s="36"/>
+      <c r="C84" s="36"/>
+      <c r="D84" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="80">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="A6:A12"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="A13:A19"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="A84:D84"/>
+    <mergeCell ref="A76:A82"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B82:D82"/>
+    <mergeCell ref="A69:A75"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="A62:A68"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="A55:A61"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B54:D54"/>
     <mergeCell ref="A34:A40"/>
     <mergeCell ref="B34:C34"/>
     <mergeCell ref="B42:C42"/>
@@ -1981,42 +2048,38 @@
     <mergeCell ref="B44:C44"/>
     <mergeCell ref="B45:C45"/>
     <mergeCell ref="B47:D47"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="A55:A61"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B61:D61"/>
-    <mergeCell ref="A62:A68"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="A69:A75"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B75:D75"/>
-    <mergeCell ref="A84:D84"/>
-    <mergeCell ref="A76:A82"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B82:D82"/>
+    <mergeCell ref="A27:A33"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="A13:A19"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="A6:A12"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B12:D12"/>
   </mergeCells>
   <conditionalFormatting sqref="D6:D11">
     <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="Terminé">
@@ -2344,15 +2407,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="8afaa137-8a18-4908-97f4-35fc924e5a91">
@@ -2361,6 +2415,15 @@
     <TaxCatchAll xmlns="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2383,14 +2446,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8C0AFF7-6D45-4588-A3CE-0506D82134A8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1CED954-0C0B-4246-88BC-C0C5C061E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -2401,4 +2456,12 @@
     <ds:schemaRef ds:uri="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8C0AFF7-6D45-4588-A3CE-0506D82134A8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>